<commit_message>
Changed parameter names in the test input sheets.
</commit_message>
<xml_diff>
--- a/test_files/data-samples/Input_4_gene_testing.xlsx
+++ b/test_files/data-samples/Input_4_gene_testing.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640" tabRatio="644"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="644" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -20,7 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">network!$A$1:$V$22</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -114,20 +119,20 @@
     <t>Sigmoid</t>
   </si>
   <si>
-    <t>iestimate</t>
-  </si>
-  <si>
-    <t>igraph</t>
-  </si>
-  <si>
     <t>dcin5</t>
+  </si>
+  <si>
+    <t>estimateParams</t>
+  </si>
+  <si>
+    <t>makeGraphs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -540,21 +545,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="13">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -568,7 +573,7 @@
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="13">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -580,7 +585,7 @@
       </c>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -592,7 +597,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="13">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -605,7 +610,7 @@
       <c r="E4" s="5"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="13">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -618,105 +623,105 @@
       <c r="E5" s="5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="13">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="4"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="13">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="4"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="13">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" s="4"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="13">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="4"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="13">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="4"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="13">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" s="4"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="13">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" s="4"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="13">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" s="4"/>
       <c r="E13" s="5"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="13">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" s="4"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="13">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" s="4"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="13">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" s="4"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="13">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="4"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="13">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18" s="4"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="13">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" s="4"/>
       <c r="E19" s="5"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="13">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20" s="4"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="13">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="13">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -728,23 +733,28 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="1"/>
   </cols>
@@ -760,7 +770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="13">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -771,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -782,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="13">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -793,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" ht="13">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -804,87 +814,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="13">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" ht="13">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="13">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" ht="13">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="13">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" ht="13">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" ht="13">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="13">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="13">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="13">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" ht="13">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" ht="13">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="13">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="13">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" ht="13">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" ht="13">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="13">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -892,20 +902,25 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
@@ -1174,18 +1189,23 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
@@ -1474,37 +1494,42 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9" style="4"/>
+    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1595,38 +1620,43 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -1734,22 +1764,27 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1830,7 +1865,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -1838,7 +1873,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -1882,7 +1917,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1910,20 +1945,25 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
@@ -1996,18 +2036,23 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
@@ -2055,5 +2100,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GRNmodel can work with files in different directories.
</commit_message>
<xml_diff>
--- a/test_files/data-samples/Input_4_gene_testing.xlsx
+++ b/test_files/data-samples/Input_4_gene_testing.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="644" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -14,8 +14,7 @@
     <sheet name="network" sheetId="5" r:id="rId5"/>
     <sheet name="network_weights" sheetId="11" r:id="rId6"/>
     <sheet name="optimization_parameters" sheetId="6" r:id="rId7"/>
-    <sheet name="simulation_times" sheetId="14" r:id="rId8"/>
-    <sheet name="network_b" sheetId="16" r:id="rId9"/>
+    <sheet name="network_b" sheetId="16" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">network!$A$1:$V$22</definedName>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t>CIN5</t>
   </si>
@@ -281,6 +280,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -575,14 +579,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -596,7 +600,7 @@
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8" ht="13">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -608,7 +612,7 @@
       </c>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" ht="13">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -620,7 +624,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" ht="13">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -633,7 +637,7 @@
       <c r="E4" s="5"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" ht="13">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -646,111 +650,111 @@
       <c r="E5" s="5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" ht="13">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="4"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" ht="13">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="4"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" ht="13">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" s="4"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" ht="13">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="4"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" ht="13">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="4"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" ht="13">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" s="4"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" ht="13">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" s="4"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:8" ht="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" s="4"/>
       <c r="E13" s="5"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8" ht="13">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" s="4"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8" ht="13">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" s="4"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" ht="13">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" s="4"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" ht="13">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="4"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" ht="13">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18" s="4"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="13">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" s="4"/>
       <c r="E19" s="5"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" ht="13">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20" s="4"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" ht="13">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" ht="13">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="H22"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E24" s="5"/>
     </row>
   </sheetData>
@@ -774,15 +778,15 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -793,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -804,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -815,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -826,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -837,87 +841,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="13">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="13">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="13">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="13">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="13">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="13">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="13">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="13">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="13">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="13">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="13">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="13">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="1:3" ht="13">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3" ht="13">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="1:3" ht="13">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -943,9 +947,9 @@
       <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -992,7 +996,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1039,7 +1043,7 @@
         <v>-1.2219770014641</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>-0.48651707588210702</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>1.55526169350673</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1180,31 +1184,31 @@
         <v>-0.19414868863404999</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G6" s="2"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J10" s="2"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G12" s="2"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="18" spans="4:13">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
       <c r="I18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="4:13">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:13">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
       <c r="F20" s="2"/>
       <c r="M20" s="2"/>
     </row>
@@ -1228,9 +1232,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1277,7 +1281,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1324,7 +1328,7 @@
         <v>-1.2219770014641</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>-0.48651707588210702</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1418,7 +1422,7 @@
         <v>1.55526169350673</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1465,51 +1469,51 @@
         <v>-0.19414868863404999</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L7" s="2"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C15" s="2"/>
     </row>
-    <row r="18" spans="7:14">
+    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="7:14">
+    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
       <c r="I19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="7:14">
+    <row r="20" spans="7:14" x14ac:dyDescent="0.2">
       <c r="I20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="22" spans="7:14">
+    <row r="22" spans="7:14" x14ac:dyDescent="0.2">
       <c r="L22" s="2"/>
       <c r="N22" s="2"/>
     </row>
@@ -1533,29 +1537,29 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.7109375" style="4"/>
+    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.75" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1572,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1589,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1606,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1661,28 +1665,28 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1716,7 +1720,7 @@
       <c r="U1"/>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1733,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1767,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1801,16 +1805,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1830,7 +1834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1854,7 +1858,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1886,23 +1890,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1932,7 +1936,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1943,7 +1947,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2036,7 +2040,7 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2048,110 +2052,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:V1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0.1</v>
-      </c>
-      <c r="D1">
-        <v>0.2</v>
-      </c>
-      <c r="E1">
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F1">
-        <v>0.4</v>
-      </c>
-      <c r="G1">
-        <v>0.5</v>
-      </c>
-      <c r="H1">
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="I1">
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="J1">
-        <v>0.8</v>
-      </c>
-      <c r="K1">
-        <v>0.9</v>
-      </c>
-      <c r="L1">
-        <v>1</v>
-      </c>
-      <c r="M1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N1">
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="O1">
-        <v>1.3</v>
-      </c>
-      <c r="P1">
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="Q1">
-        <v>1.5</v>
-      </c>
-      <c r="R1">
-        <v>1.6</v>
-      </c>
-      <c r="S1">
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="T1">
-        <v>1.8</v>
-      </c>
-      <c r="U1">
-        <v>1.9000000000000001</v>
-      </c>
-      <c r="V1">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2159,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2167,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2175,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2183,10 +2097,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
     </row>
   </sheetData>

</xml_diff>